<commit_message>
v1 avec debut front + gitignore
</commit_message>
<xml_diff>
--- a/documentationTechnique/backend_endpoints.xlsx
+++ b/documentationTechnique/backend_endpoints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clementgardair/portfolio-monorepo/documentationTechnique/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1505671-600F-4444-9E23-895B371BC536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A4D33F-4587-C848-B988-D0AD16F3D240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="29400" windowHeight="18440" xr2:uid="{DCEA27B5-1A5E-E745-9944-F530664F706B}"/>
   </bookViews>
@@ -813,8 +813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B0F4B6D-9C97-4948-8FD9-9F9514DEAA2B}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J29" sqref="A1:J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>